<commit_message>
program 4 jeszcze niepelny
</commit_message>
<xml_diff>
--- a/zad4/MIASI-4.xlsx
+++ b/zad4/MIASI-4.xlsx
@@ -23,6 +23,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Pstr</t>
+  </si>
+  <si>
+    <t>Pobs</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>i*Pc+1</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
@@ -35,15 +88,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,12 +110,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,12 +413,487 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:Q14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>1/SUM(C5:C14)</f>
+        <v>4.2761585310537864E-3</v>
+      </c>
+      <c r="E5">
+        <f>C5*D6</f>
+        <v>6.8418536496860586E-3</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>(POWER(A6,B6))/(FACT($B$1)*POWER($B$2,B6)*POWER($B$1,B6-$B$1))</f>
+        <v>1.6</v>
+      </c>
+      <c r="D6">
+        <f>$D$5*C6</f>
+        <v>6.8418536496860586E-3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E14" si="0">C6*D7</f>
+        <v>6.5681795036986153E-3</v>
+      </c>
+      <c r="F6">
+        <f>C$21/A6</f>
+        <v>11.521541185231115</v>
+      </c>
+      <c r="P6" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>11.521541185231115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C14" si="1">(POWER(A7,B7))/(FACT($B$1)*POWER($B$2,B7)*POWER($B$1,B7-$B$1))</f>
+        <v>0.96</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D14" si="2">$D$5*C7</f>
+        <v>4.1051121898116345E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3.9901690484969096E-3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F14" si="3">C$21/A7</f>
+        <v>5.7607705926155575</v>
+      </c>
+      <c r="P7" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>5.7607705926155575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f>(POWER(A8,B8))/(FACT($B$1)*POWER($B$2,B8)*POWER($B$1,B8-$B$1))</f>
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>4.1564260921842806E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>5.7458434298355496E-3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>3.8405137284103716</v>
+      </c>
+      <c r="P8" s="2">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>3.8405137284103716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>1.3824000000000001</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>5.9113615533287547E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.4963133931863409E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>2.8803852963077787</v>
+      </c>
+      <c r="P9" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>2.8803852963077787</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f>(POWER(A10,B10))/(FACT($B$1)*POWER($B$2,B10)*POWER($B$1,B10-$B$1))</f>
+        <v>2.53125</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1.0824026281729897E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>6.1358201079347391E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>2.3043082370462229</v>
+      </c>
+      <c r="P10" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2.3043082370462229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>5.668704</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>2.4240276969618724E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.36382404233872073</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>1.9202568642051858</v>
+      </c>
+      <c r="P11" s="2">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1.9202568642051858</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>15.009071175000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>6.4181167748169732E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2.9436509183593089</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>1.6459344550330164</v>
+      </c>
+      <c r="P12" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1.6459344550330164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>45.864714239999998</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.19612478907172007</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>31.157681214352387</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>1.4401926481538894</v>
+      </c>
+      <c r="P13" s="2">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1.4401926481538894</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>158.86661427056251</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.67933882791269706</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>1.2801712428034573</v>
+      </c>
+      <c r="P14" s="2">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.2801712428034573</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <f>D14</f>
+        <v>0.67933882791269706</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>G19*D6</f>
+        <v>6.8418536496860586E-3</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f>1-C19</f>
+        <v>0.32066117208730294</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H22" si="4">G20*D7</f>
+        <v>8.2102243796232689E-3</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <f>SUM(E5:E14)</f>
+        <v>34.564623555693345</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>1.2469278276552842E-2</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <f>SUM(H19:H22)+SUM(K23:K27)</f>
+        <v>3.9500031544549192</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>2.3645446213315019E-2</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <f>C21+C22</f>
+        <v>38.514626710148264</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <f>B$1*D10</f>
+        <v>4.3296105126919587E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K27" si="5">B$1*D11</f>
+        <v>9.6961107878474895E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>7</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>0.25672467099267893</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>8</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>0.78449915628688027</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>9</v>
+      </c>
+      <c r="K27">
+        <f>B$1*D14</f>
+        <v>2.7173553116507883</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zad4: fix stany fazowe
</commit_message>
<xml_diff>
--- a/zad4/MIASI-4.xlsx
+++ b/zad4/MIASI-4.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MiASI\zad4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neufrin\Documents\MiASI\zad4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>c</t>
   </si>
@@ -92,6 +93,12 @@
   <si>
     <t>c*p</t>
   </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
 </sst>
 </file>
 
@@ -107,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,13 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,10 +183,1086 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>prawdopodobieństwo stanów fazowych </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>λ = 21 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$10:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$10:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.7491346041272824E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9946365337334588E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.188736720840263E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8642314091763688E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1574429796351873E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4653151286169469E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.788580885047793E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1280099293001831E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.4844104257651922E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8586309470534521E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2515624944061255E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.6641406191264314E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.097347650082753E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5522150325868888E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10029825784216236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-214186832"/>
+        <c:axId val="-214173232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-214186832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>i</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-214173232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-214173232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>p</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-214186832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -210,7 +1300,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -282,7 +1372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -921,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1029,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D10" si="3">POWER(B7,C7)/FACT(C7)</f>
+        <f t="shared" ref="D7:D9" si="3">POWER(B7,C7)/FACT(C7)</f>
         <v>0.6</v>
       </c>
       <c r="E7">
@@ -1286,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E7:E19" si="7">D15/SUM(D$5:D$19)</f>
+        <f t="shared" ref="E15:E19" si="7">D15/SUM(D$5:D$19)</f>
         <v>0</v>
       </c>
     </row>
@@ -1383,4 +2473,404 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <f>1/SUM(C10:C24)</f>
+        <v>4.7491346041272824E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>POWER(C$3,B10)/(FACT(B10)*POWER(C$5,B10))</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>C10*F$8</f>
+        <v>4.7491346041272824E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>POWER(C$3,B11)/(FACT(B11)*POWER(C$5,B11))</f>
+        <v>4.2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D24" si="0">C11*F$8</f>
+        <v>1.9946365337334588E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C14" si="1">POWER(C$3,B12)/(FACT(B12)*POWER(C$5,B12))</f>
+        <v>8.82</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4.188736720840263E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>12.348000000000001</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>5.8642314091763688E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>12.965400000000001</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6.1574429796351873E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f>POWER(C$3,B15)/(FACT(C$4)*POWER(C$5,B15)*(POWER(C$4,B15)/POWER(C$4,C$4)))</f>
+        <v>13.613670000000001</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.4653151286169469E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C24" si="2">POWER(C$3,B16)/(FACT(C$4)*POWER(C$5,B16)*(POWER(C$4,B16)/POWER(C$4,C$4)))</f>
+        <v>14.2943535</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6.788580885047793E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>15.009071175000001</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>7.1280099293001831E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>15.75952473375</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>7.4844104257651922E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>16.5475009704375</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>7.8586309470534521E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>17.374876018959377</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>8.2515624944061255E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>18.243619819907344</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>8.6641406191264314E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>19.155800810902711</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>9.097347650082753E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>20.113590851447846</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>9.5522150325868888E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>21.119270394020241</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.10029825784216236</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>SUM(D10:D24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.7491346041272824E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.9946365337334588E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>4.188736720840263E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>5.8642314091763688E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6.1574429796351873E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <v>5</v>
+      </c>
+      <c r="D39" s="2">
+        <v>6.4653151286169469E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2">
+        <v>6.788580885047793E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <v>7</v>
+      </c>
+      <c r="D41" s="2">
+        <v>7.1280099293001831E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2">
+        <v>7.4844104257651922E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <v>9</v>
+      </c>
+      <c r="D43" s="2">
+        <v>7.8586309470534521E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <v>10</v>
+      </c>
+      <c r="D44" s="2">
+        <v>8.2515624944061255E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <v>11</v>
+      </c>
+      <c r="D45" s="2">
+        <v>8.6641406191264314E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <v>12</v>
+      </c>
+      <c r="D46" s="2">
+        <v>9.097347650082753E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2">
+        <v>9.5522150325868888E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <v>14</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.10029825784216236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>